<commit_message>
updated excel sheet(sheet name=HrHeadEmployee),edited HrHeadAddEmployee test script
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData.xlsx
+++ b/src/test/resources/TestData.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent>
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f68878467098e075/Desktop/personal finance project/com.intelli.hrm.framework/src/test/resources/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="3" documentId="11_4309D94FA18114FA8A0027784D9B6C815253FF7F" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AE8130EC-A3A0-40E5-B9B1-63246F5989D3}"/>
   <bookViews>
-    <workbookView xWindow="600" yWindow="360" windowWidth="19695" windowHeight="7665" activeTab="4"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Branches" sheetId="1" r:id="rId1"/>
@@ -18,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="39">
   <si>
     <t>TestCaseName</t>
   </si>
@@ -53,9 +59,6 @@
     <t>username</t>
   </si>
   <si>
-    <t>hrhead@gmail.com</t>
-  </si>
-  <si>
     <t>CorporateName</t>
   </si>
   <si>
@@ -132,13 +135,20 @@
   </si>
   <si>
     <t>875-535-33</t>
+  </si>
+  <si>
+    <t>pass</t>
+  </si>
+  <si>
+    <t>emil</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -281,15 +291,9 @@
   <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="49" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
@@ -307,6 +311,12 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="49" fontId="0" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -320,6 +330,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -366,7 +384,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -398,9 +416,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -432,6 +468,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -607,42 +661,42 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="14.26953125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="18.26953125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3" t="s">
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
-      <c r="A2" s="3"/>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2" s="16"/>
       <c r="B2" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
-      <c r="E2" s="3"/>
-    </row>
-    <row r="3" spans="1:5">
+      <c r="E2" s="16"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -655,7 +709,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
@@ -677,41 +731,41 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="14.26953125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3" t="s">
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
-      <c r="A2" s="3"/>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2" s="16"/>
       <c r="B2" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
-      <c r="E2" s="3"/>
-    </row>
-    <row r="3" spans="1:5">
+      <c r="E2" s="16"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
@@ -735,50 +789,53 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="20.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="20.7265625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="17.36328125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="6.453125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3" t="s">
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
-      <c r="A2" s="3"/>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2" s="16"/>
       <c r="B2" s="2" t="s">
         <v>10</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
-      <c r="E2" s="3"/>
-    </row>
-    <row r="3" spans="1:5">
+      <c r="E2" s="16"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="4" t="s">
-        <v>11</v>
+      <c r="B3" s="3" t="s">
+        <v>38</v>
       </c>
       <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
+      <c r="D3" s="1" t="s">
+        <v>37</v>
+      </c>
       <c r="E3" s="1" t="s">
         <v>5</v>
       </c>
@@ -790,113 +847,113 @@
     <mergeCell ref="E1:E2"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="B3" r:id="rId1"/>
+    <hyperlink ref="B3" r:id="rId1" display="hrhead@gmail.com" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="19.81640625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="10.1796875" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="9.7265625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="12.7265625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="12.54296875" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="7" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="A2" s="8" t="s">
+      <c r="B2" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="C2" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="D2" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="D2" s="10" t="s">
+      <c r="E2" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="E2" s="11" t="s">
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3" s="10"/>
+      <c r="B3" s="6" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" s="12"/>
-      <c r="B3" s="8" t="s">
+      <c r="C3" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="D3" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="D3" s="13" t="s">
+      <c r="E3" s="12"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4" s="10"/>
+      <c r="B4" s="6"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="11"/>
+      <c r="E4" s="12"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="E3" s="14"/>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" s="12"/>
-      <c r="B4" s="8"/>
-      <c r="C4" s="8"/>
-      <c r="D4" s="13"/>
-      <c r="E4" s="14"/>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" s="15" t="s">
+      <c r="B5" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" s="12"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A6" s="10"/>
+      <c r="B6" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="B5" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="D5" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="E5" s="14"/>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="A6" s="12"/>
-      <c r="B6" s="8" t="s">
+      <c r="C6" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="D6" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="D6" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="E6" s="14"/>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="A7" s="15"/>
-      <c r="B7" s="8"/>
-      <c r="C7" s="8"/>
-      <c r="D7" s="13"/>
-      <c r="E7" s="16"/>
+      <c r="E6" s="12"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A7" s="13"/>
+      <c r="B7" s="6"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="11"/>
+      <c r="E7" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -907,30 +964,30 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="19.7265625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="12.81640625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="15.1796875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="11.453125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="12.54296875" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="9.453125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="10.453125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
-      <c r="A1" s="17" t="s">
-        <v>13</v>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A1" s="15" t="s">
+        <v>12</v>
       </c>
       <c r="B1" s="18" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C1" s="19"/>
       <c r="D1" s="19"/>
@@ -938,58 +995,58 @@
       <c r="F1" s="19"/>
       <c r="G1" s="19"/>
     </row>
-    <row r="2" spans="1:7">
-      <c r="A2" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="B2" s="9" t="s">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A2" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="D2" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="E2" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="F2" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="E2" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="F2" s="9" t="s">
+      <c r="G2" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="G2" s="9" t="s">
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A3" s="6"/>
+      <c r="B3" s="6" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="3" spans="1:7">
-      <c r="A3" s="8"/>
-      <c r="B3" s="8" t="s">
+      <c r="C3" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="D3" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="E3" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="E3" s="8" t="s">
+      <c r="F3" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="F3" s="8" t="s">
+      <c r="G3" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="G3" s="8" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
-      <c r="A4" s="8"/>
-      <c r="B4" s="8"/>
-      <c r="C4" s="8"/>
-      <c r="D4" s="8"/>
-      <c r="E4" s="8"/>
-      <c r="F4" s="8"/>
-      <c r="G4" s="8"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A4" s="6"/>
+      <c r="B4" s="6"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
This is full hrm project-venkat
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData.xlsx
+++ b/src/test/resources/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="600" yWindow="360" windowWidth="19695" windowHeight="7665" activeTab="4"/>
+    <workbookView xWindow="600" yWindow="360" windowWidth="19695" windowHeight="7665" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Branches" sheetId="1" r:id="rId1"/>
@@ -12,13 +12,14 @@
     <sheet name="HRHeadEmployee" sheetId="3" r:id="rId3"/>
     <sheet name="EmployeeDetails" sheetId="4" r:id="rId4"/>
     <sheet name="EmployeeContact" sheetId="5" r:id="rId5"/>
+    <sheet name="AdminDetails" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="55">
   <si>
     <t>TestCaseName</t>
   </si>
@@ -132,13 +133,64 @@
   </si>
   <si>
     <t>875-535-33</t>
+  </si>
+  <si>
+    <t>AddAdminTest</t>
+  </si>
+  <si>
+    <t>Company ID</t>
+  </si>
+  <si>
+    <t>First Name</t>
+  </si>
+  <si>
+    <t>Last Name</t>
+  </si>
+  <si>
+    <t>Middle Name</t>
+  </si>
+  <si>
+    <t>Contact No</t>
+  </si>
+  <si>
+    <t>Email Address</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>EN921</t>
+  </si>
+  <si>
+    <t>Sathya</t>
+  </si>
+  <si>
+    <t>Moorthy</t>
+  </si>
+  <si>
+    <t>sathya@gmail.com</t>
+  </si>
+  <si>
+    <t>sathya@123</t>
+  </si>
+  <si>
+    <t>K</t>
+  </si>
+  <si>
+    <t>09876543210</t>
+  </si>
+  <si>
+    <t>Postion</t>
+  </si>
+  <si>
+    <t>→ HR Head</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -157,6 +209,14 @@
       <b/>
       <sz val="11"/>
       <color rgb="FF7030A0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="7" tint="-0.249977111117893"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -278,18 +338,12 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="49" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
@@ -307,12 +361,22 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="49" fontId="0" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -621,26 +685,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3" t="s">
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="3"/>
+      <c r="A2" s="16"/>
       <c r="B2" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
-      <c r="E2" s="3"/>
+      <c r="E2" s="16"/>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="1" t="s">
@@ -690,26 +754,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3" t="s">
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="3"/>
+      <c r="A2" s="16"/>
       <c r="B2" s="2" t="s">
         <v>12</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
-      <c r="E2" s="3"/>
+      <c r="E2" s="16"/>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="1" t="s">
@@ -749,32 +813,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3" t="s">
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="3"/>
+      <c r="A2" s="16"/>
       <c r="B2" s="2" t="s">
         <v>10</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
-      <c r="E2" s="3"/>
+      <c r="E2" s="16"/>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="3" t="s">
         <v>11</v>
       </c>
       <c r="C3" s="1"/>
@@ -801,7 +865,7 @@
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -814,89 +878,89 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="7" t="s">
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="5" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="C2" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="D2" s="10" t="s">
+      <c r="D2" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="E2" s="11" t="s">
+      <c r="E2" s="9" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:5">
-      <c r="A3" s="12"/>
-      <c r="B3" s="8" t="s">
+      <c r="A3" s="10"/>
+      <c r="B3" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="D3" s="13" t="s">
+      <c r="D3" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="E3" s="14"/>
+      <c r="E3" s="12"/>
     </row>
     <row r="4" spans="1:5">
-      <c r="A4" s="12"/>
-      <c r="B4" s="8"/>
-      <c r="C4" s="8"/>
-      <c r="D4" s="13"/>
-      <c r="E4" s="14"/>
+      <c r="A4" s="10"/>
+      <c r="B4" s="6"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="11"/>
+      <c r="E4" s="12"/>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5" s="15" t="s">
+      <c r="A5" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="B5" s="9" t="s">
+      <c r="B5" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="9" t="s">
+      <c r="C5" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="10" t="s">
+      <c r="D5" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="E5" s="14"/>
+      <c r="E5" s="12"/>
     </row>
     <row r="6" spans="1:5">
-      <c r="A6" s="12"/>
-      <c r="B6" s="8" t="s">
+      <c r="A6" s="10"/>
+      <c r="B6" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="C6" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="D6" s="13" t="s">
+      <c r="D6" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="E6" s="14"/>
+      <c r="E6" s="12"/>
     </row>
     <row r="7" spans="1:5">
-      <c r="A7" s="15"/>
-      <c r="B7" s="8"/>
-      <c r="C7" s="8"/>
-      <c r="D7" s="13"/>
-      <c r="E7" s="16"/>
+      <c r="A7" s="13"/>
+      <c r="B7" s="6"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="11"/>
+      <c r="E7" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -910,8 +974,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -926,7 +990,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="15" t="s">
         <v>13</v>
       </c>
       <c r="B1" s="18" t="s">
@@ -939,57 +1003,57 @@
       <c r="G1" s="19"/>
     </row>
     <row r="2" spans="1:7">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="C2" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="D2" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="E2" s="9" t="s">
+      <c r="E2" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="F2" s="9" t="s">
+      <c r="F2" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="G2" s="9" t="s">
+      <c r="G2" s="7" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:7">
-      <c r="A3" s="8"/>
-      <c r="B3" s="8" t="s">
+      <c r="A3" s="6"/>
+      <c r="B3" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="D3" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="E3" s="8" t="s">
+      <c r="E3" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="F3" s="8" t="s">
+      <c r="F3" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="G3" s="8" t="s">
+      <c r="G3" s="6" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:7">
-      <c r="A4" s="8"/>
-      <c r="B4" s="8"/>
-      <c r="C4" s="8"/>
-      <c r="D4" s="8"/>
-      <c r="E4" s="8"/>
-      <c r="F4" s="8"/>
-      <c r="G4" s="8"/>
+      <c r="A4" s="6"/>
+      <c r="B4" s="6"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -997,4 +1061,117 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:I4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="11.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9">
+      <c r="A1" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="20"/>
+      <c r="I1" s="20"/>
+    </row>
+    <row r="2" spans="1:9">
+      <c r="A2" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="G2" s="23" t="s">
+        <v>53</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="I2" s="21" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3" s="6"/>
+      <c r="B3" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="C3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="H3" s="22" t="s">
+        <v>49</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4" s="6"/>
+      <c r="B4" s="6"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="6"/>
+      <c r="I4" s="1"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B1:G1"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="H3" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>